<commit_message>
using film code instead of titleId
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
@@ -40,7 +40,38 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Title ID 1</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Film Code 1 
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">internal</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> reference, same as other excel import)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Distribution IDs 1</t>
@@ -58,7 +89,38 @@
     <t xml:space="preserve">Fees currency 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Title ID 2</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Film Code 2 
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">internal</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> reference, same as other excel import)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Distribution IDs 2</t>
@@ -83,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -112,6 +174,21 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -181,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,7 +267,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,8 +362,8 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,10 +378,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="29.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="12" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.65"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -318,37 +403,37 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[WIP] #1562  new excel movie (#1598)
* [WIP] #1562

* new template for movies

* cleaning old comments

* first pass for contracts

* debug

* fixed circular dependency issue

* debug ok

* working contracts import

* happy linter

* linter debug
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Contracts" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,12 +20,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">Licensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licensee</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+  <si>
+    <t xml:space="preserve">Licensor (name, &lt;orgId&gt;)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Licensee</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (name, &lt;orgId&gt;)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Child Roles (name, role, role,..)</t>
   </si>
   <si>
     <t xml:space="preserve">Contract ID</t>
@@ -40,15 +63,29 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Film Code 1 
+    <t xml:space="preserve">Creation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope Start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope End date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment schedules
+(label. percentage, date)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Film Code 1
 (</t>
     </r>
     <r>
@@ -59,6 +96,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">internal</t>
     </r>
@@ -69,6 +107,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> reference, same as other excel import)</t>
     </r>
@@ -96,6 +135,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Film Code 2 
 (</t>
@@ -108,6 +148,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">internal</t>
     </r>
@@ -118,6 +159,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> reference, same as other excel import)</t>
     </r>
@@ -136,6 +178,214 @@
   </si>
   <si>
     <t xml:space="preserve">Fees currency 2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Film Code 3
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">internal</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> reference, same as other excel import)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution IDs 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commission 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees label 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees value 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees currency 3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Film Code 4
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">internal</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> reference, same as other excel import)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution IDs 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commission 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees label 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees value 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees currency 4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Film Code 5
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">internal</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> reference, same as other excel import)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution IDs 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commission 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees label 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees value 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees currency 5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Film Code 6
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">internal</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> reference, same as other excel import)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution IDs 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commission 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees label 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees value 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees currency 6</t>
   </si>
 </sst>
 </file>
@@ -189,6 +439,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -258,7 +509,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,15 +518,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,28 +607,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="12" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="0" width="29.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="17" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="10.65"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="80.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,41 +647,128 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -466,8 +800,6 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Feat 1872 - public contract collection & feat-1653 debug/update import (#1885)
* feat-1653

* feat-1872 & debug feat-1653

* debug

* linter

* more verbose comments

* update after review

* debug

* debug after review
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
@@ -20,38 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Licensor (name, &lt;orgId&gt;)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Licensee</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (name, &lt;orgId&gt;)</t>
-    </r>
+    <t xml:space="preserve">Licensee (name, &lt;orgId&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">Child Roles (name, role, role,..)</t>
   </si>
   <si>
     <t xml:space="preserve">Contract ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract Type (Mandate, Sale)</t>
   </si>
   <si>
     <t xml:space="preserve">Parent Contract ID</t>
@@ -395,7 +378,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -424,13 +407,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -607,10 +583,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:AV2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,7 +604,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="10.65"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="80.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +626,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -662,7 +638,7 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
@@ -680,7 +656,7 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -698,7 +674,7 @@
       <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="3" t="s">
@@ -716,7 +692,7 @@
       <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="4" t="s">
@@ -734,7 +710,7 @@
       <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="AK1" s="3" t="s">
@@ -752,7 +728,7 @@
       <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="3" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="4" t="s">
@@ -769,6 +745,9 @@
       </c>
       <c r="AU1" s="4" t="s">
         <v>46</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
moved title price from sales to contract file
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Licensor (name, &lt;orgId&gt;)</t>
   </si>
@@ -99,6 +99,10 @@
     <t xml:space="preserve">Distribution IDs 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 1
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 1</t>
   </si>
   <si>
@@ -151,6 +155,10 @@
     <t xml:space="preserve">Distribution IDs 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 2
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 2</t>
   </si>
   <si>
@@ -203,6 +211,10 @@
     <t xml:space="preserve">Distribution IDs 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 3
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 3</t>
   </si>
   <si>
@@ -255,6 +267,10 @@
     <t xml:space="preserve">Distribution IDs 4</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 4
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 4</t>
   </si>
   <si>
@@ -307,6 +323,10 @@
     <t xml:space="preserve">Distribution IDs 5</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 5
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 5</t>
   </si>
   <si>
@@ -359,6 +379,10 @@
     <t xml:space="preserve">Distribution IDs 6</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 6
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 6</t>
   </si>
   <si>
@@ -369,6 +393,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fees currency 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(amount, currency)</t>
   </si>
 </sst>
 </file>
@@ -378,7 +405,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -416,6 +443,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -485,7 +519,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -502,8 +536,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -583,13 +629,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AX2" activeCellId="0" sqref="AX2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.83"/>
@@ -599,12 +645,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="0" width="29.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="17" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="18" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="10.65"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="80.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +693,7 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -659,28 +705,28 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="3" t="s">
@@ -689,40 +735,40 @@
       <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="5" t="s">
         <v>39</v>
       </c>
       <c r="AO1" s="3" t="s">
@@ -734,51 +780,45 @@
       <c r="AQ1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="AW1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AJ2" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
moved column & updated price
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
@@ -20,12 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Licensor (name, &lt;orgId&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">Licensee (name, &lt;orgId&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to show the operator name on a buyer research ?
+(Yes or No)</t>
   </si>
   <si>
     <t xml:space="preserve">Child Roles (name, role, role,..)</t>
@@ -437,19 +441,19 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -519,12 +523,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,19 +544,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -629,25 +629,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB2"/>
+  <dimension ref="A1:BC2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AX2" activeCellId="0" sqref="AX2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="18" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="42.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="0" width="29.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="40.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="15" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="19" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,7 +657,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -675,46 +675,46 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="5" t="s">
@@ -729,34 +729,34 @@
       <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
       <c r="AI1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>35</v>
       </c>
       <c r="AK1" s="5" t="s">
@@ -771,34 +771,34 @@
       <c r="AN1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="4" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AS1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AV1" s="4" t="s">
         <v>47</v>
       </c>
       <c r="AW1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="5" t="s">
         <v>49</v>
       </c>
       <c r="AY1" s="5" t="s">
@@ -813,10 +813,13 @@
       <c r="BB1" s="5" t="s">
         <v>53</v>
       </c>
+      <c r="BC1" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AJ2" s="7" t="s">
-        <v>54</v>
+      <c r="AK2" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat 1955 - Excel import: improvements (#2083)
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
@@ -20,12 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Licensor (name, &lt;orgId&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">Licensee (name, &lt;orgId&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to show the operator name on a buyer research ?
+(Yes or No)</t>
   </si>
   <si>
     <t xml:space="preserve">Child Roles (name, role, role,..)</t>
@@ -99,6 +103,10 @@
     <t xml:space="preserve">Distribution IDs 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 1
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 1</t>
   </si>
   <si>
@@ -151,6 +159,10 @@
     <t xml:space="preserve">Distribution IDs 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 2
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 2</t>
   </si>
   <si>
@@ -203,6 +215,10 @@
     <t xml:space="preserve">Distribution IDs 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 3
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 3</t>
   </si>
   <si>
@@ -255,6 +271,10 @@
     <t xml:space="preserve">Distribution IDs 4</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 4
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 4</t>
   </si>
   <si>
@@ -307,6 +327,10 @@
     <t xml:space="preserve">Distribution IDs 5</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 5
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 5</t>
   </si>
   <si>
@@ -359,6 +383,10 @@
     <t xml:space="preserve">Distribution IDs 6</t>
   </si>
   <si>
+    <t xml:space="preserve">Global price 6
+(amount, currency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commission 6</t>
   </si>
   <si>
@@ -369,6 +397,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fees currency 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(amount, currency)</t>
   </si>
 </sst>
 </file>
@@ -378,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -407,6 +438,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -485,12 +523,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,6 +546,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -583,35 +629,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:BC2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="17" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="42.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="0" width="29.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="40.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="15" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="19" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="10.65"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="80.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -629,34 +675,34 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -665,34 +711,34 @@
       <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="4" t="s">
@@ -707,28 +753,28 @@
       <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="4" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="4" t="s">
@@ -749,36 +795,33 @@
       <c r="AV1" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="AW1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AK2" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Feat 1887 ter - front cleaning (#2292)
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-contracts-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Licensor (name, &lt;orgId&gt;)</t>
   </si>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t xml:space="preserve">Contract Type (Mandate, Sale)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent Contract ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chid Contract ID</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -409,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -438,13 +432,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -523,16 +510,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -629,10 +612,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BA2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -641,23 +624,23 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="29.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="42.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="40.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="15" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="19" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="29.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="40.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="17" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="25" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="80.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -672,16 +655,16 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -690,19 +673,19 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -711,40 +694,40 @@
       <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="4" t="s">
@@ -753,40 +736,40 @@
       <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AN1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="3" t="s">
         <v>45</v>
       </c>
       <c r="AU1" s="4" t="s">
@@ -795,31 +778,25 @@
       <c r="AV1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AX1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AY1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="BB1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AK2" s="6" t="s">
-        <v>55</v>
+      <c r="AI2" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>